<commit_message>
// summation was optimized.
</commit_message>
<xml_diff>
--- a/src/main/resources/cpu vs gpu.xlsx
+++ b/src/main/resources/cpu vs gpu.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ccivi\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ccivi\Desktop\cpu vs gpu\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CD242DA-DAF8-4838-99C0-C00EEF5ABB6B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB00BD6E-F825-4C55-8CAD-5C5B2A827412}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5790" yWindow="225" windowWidth="21600" windowHeight="11385" xr2:uid="{BD9A81EE-2658-493F-8908-11A4B8217F53}"/>
   </bookViews>
@@ -303,10 +303,10 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
                   <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>0</c:v>
@@ -315,16 +315,16 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>3</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>11</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>41</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>169</c:v>
+                  <c:v>208</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -412,46 +412,46 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="28"/>
                 <c:pt idx="0">
-                  <c:v>528</c:v>
+                  <c:v>672</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>106</c:v>
+                  <c:v>83</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>122</c:v>
+                  <c:v>89</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>105</c:v>
+                  <c:v>74</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>102</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>121</c:v>
+                  <c:v>97</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>124</c:v>
+                  <c:v>76</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>130</c:v>
+                  <c:v>97</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>143</c:v>
+                  <c:v>110</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>180</c:v>
+                  <c:v>105</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>296</c:v>
+                  <c:v>135</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>567</c:v>
+                  <c:v>196</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>1627</c:v>
+                  <c:v>323</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>5651</c:v>
+                  <c:v>936</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7144,8 +7144,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83F6B179-546E-4BBF-8771-C763CFAAE407}">
   <dimension ref="A1:D145"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A112" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="T128" sqref="T128"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7181,7 +7181,7 @@
         <v>0</v>
       </c>
       <c r="D2">
-        <v>528</v>
+        <v>672</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -7196,7 +7196,7 @@
         <v>0</v>
       </c>
       <c r="D3">
-        <v>106</v>
+        <v>83</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -7211,7 +7211,7 @@
         <v>0</v>
       </c>
       <c r="D4">
-        <v>122</v>
+        <v>89</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -7226,7 +7226,7 @@
         <v>0</v>
       </c>
       <c r="D5">
-        <v>105</v>
+        <v>74</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -7256,7 +7256,7 @@
         <v>0</v>
       </c>
       <c r="D7">
-        <v>121</v>
+        <v>97</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -7268,10 +7268,10 @@
         <v>16384</v>
       </c>
       <c r="C8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D8">
-        <v>124</v>
+        <v>76</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -7283,10 +7283,10 @@
         <v>65536</v>
       </c>
       <c r="C9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D9">
-        <v>130</v>
+        <v>97</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -7301,7 +7301,7 @@
         <v>0</v>
       </c>
       <c r="D10">
-        <v>143</v>
+        <v>110</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -7316,7 +7316,7 @@
         <v>1</v>
       </c>
       <c r="D11">
-        <v>180</v>
+        <v>105</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -7328,10 +7328,10 @@
         <v>4194304</v>
       </c>
       <c r="C12">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D12" s="1">
-        <v>296</v>
+        <v>135</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -7343,10 +7343,10 @@
         <v>16777216</v>
       </c>
       <c r="C13">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D13" s="1">
-        <v>567</v>
+        <v>196</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -7361,7 +7361,7 @@
         <v>41</v>
       </c>
       <c r="D14" s="1">
-        <v>1627</v>
+        <v>323</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -7373,10 +7373,10 @@
         <v>268435456</v>
       </c>
       <c r="C15">
-        <v>169</v>
+        <v>208</v>
       </c>
       <c r="D15" s="1">
-        <v>5651</v>
+        <v>936</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -8194,7 +8194,7 @@
         <v>2</v>
       </c>
       <c r="B92">
-        <f t="shared" ref="B92:B118" si="3">2^A92</f>
+        <f t="shared" ref="B92:B115" si="3">2^A92</f>
         <v>4</v>
       </c>
       <c r="C92">
@@ -8565,7 +8565,7 @@
         <v>1</v>
       </c>
       <c r="B122">
-        <f>2^A122</f>
+        <f t="shared" ref="B122:B143" si="4">2^A122</f>
         <v>2</v>
       </c>
       <c r="C122">
@@ -8580,7 +8580,7 @@
         <v>2</v>
       </c>
       <c r="B123">
-        <f>2^A123</f>
+        <f t="shared" si="4"/>
         <v>4</v>
       </c>
       <c r="C123">
@@ -8595,7 +8595,7 @@
         <v>3</v>
       </c>
       <c r="B124">
-        <f>2^A124</f>
+        <f t="shared" si="4"/>
         <v>8</v>
       </c>
       <c r="C124">
@@ -8610,7 +8610,7 @@
         <v>4</v>
       </c>
       <c r="B125">
-        <f>2^A125</f>
+        <f t="shared" si="4"/>
         <v>16</v>
       </c>
       <c r="C125">
@@ -8625,7 +8625,7 @@
         <v>5</v>
       </c>
       <c r="B126">
-        <f>2^A126</f>
+        <f t="shared" si="4"/>
         <v>32</v>
       </c>
       <c r="C126">
@@ -8640,7 +8640,7 @@
         <v>6</v>
       </c>
       <c r="B127">
-        <f>2^A127</f>
+        <f t="shared" si="4"/>
         <v>64</v>
       </c>
       <c r="C127">
@@ -8655,7 +8655,7 @@
         <v>7</v>
       </c>
       <c r="B128">
-        <f>2^A128</f>
+        <f t="shared" si="4"/>
         <v>128</v>
       </c>
       <c r="C128">
@@ -8670,7 +8670,7 @@
         <v>8</v>
       </c>
       <c r="B129">
-        <f>2^A129</f>
+        <f t="shared" si="4"/>
         <v>256</v>
       </c>
       <c r="C129">
@@ -8685,7 +8685,7 @@
         <v>9</v>
       </c>
       <c r="B130">
-        <f>2^A130</f>
+        <f t="shared" si="4"/>
         <v>512</v>
       </c>
       <c r="C130">
@@ -8700,7 +8700,7 @@
         <v>10</v>
       </c>
       <c r="B131">
-        <f>2^A131</f>
+        <f t="shared" si="4"/>
         <v>1024</v>
       </c>
       <c r="C131">
@@ -8715,7 +8715,7 @@
         <v>11</v>
       </c>
       <c r="B132">
-        <f>2^A132</f>
+        <f t="shared" si="4"/>
         <v>2048</v>
       </c>
       <c r="C132">
@@ -8730,7 +8730,7 @@
         <v>12</v>
       </c>
       <c r="B133">
-        <f>2^A133</f>
+        <f t="shared" si="4"/>
         <v>4096</v>
       </c>
       <c r="C133">
@@ -8745,7 +8745,7 @@
         <v>13</v>
       </c>
       <c r="B134">
-        <f>2^A134</f>
+        <f t="shared" si="4"/>
         <v>8192</v>
       </c>
       <c r="C134">
@@ -8760,7 +8760,7 @@
         <v>14</v>
       </c>
       <c r="B135">
-        <f>2^A135</f>
+        <f t="shared" si="4"/>
         <v>16384</v>
       </c>
       <c r="C135">
@@ -8775,7 +8775,7 @@
         <v>15</v>
       </c>
       <c r="B136">
-        <f>2^A136</f>
+        <f t="shared" si="4"/>
         <v>32768</v>
       </c>
       <c r="C136">
@@ -8790,7 +8790,7 @@
         <v>16</v>
       </c>
       <c r="B137">
-        <f>2^A137</f>
+        <f t="shared" si="4"/>
         <v>65536</v>
       </c>
       <c r="C137">
@@ -8805,7 +8805,7 @@
         <v>17</v>
       </c>
       <c r="B138">
-        <f>2^A138</f>
+        <f t="shared" si="4"/>
         <v>131072</v>
       </c>
       <c r="C138">
@@ -8820,7 +8820,7 @@
         <v>18</v>
       </c>
       <c r="B139">
-        <f>2^A139</f>
+        <f t="shared" si="4"/>
         <v>262144</v>
       </c>
       <c r="C139">
@@ -8835,7 +8835,7 @@
         <v>19</v>
       </c>
       <c r="B140">
-        <f>2^A140</f>
+        <f t="shared" si="4"/>
         <v>524288</v>
       </c>
       <c r="C140">
@@ -8850,7 +8850,7 @@
         <v>20</v>
       </c>
       <c r="B141">
-        <f>2^A141</f>
+        <f t="shared" si="4"/>
         <v>1048576</v>
       </c>
       <c r="D141">
@@ -8862,7 +8862,7 @@
         <v>21</v>
       </c>
       <c r="B142">
-        <f>2^A142</f>
+        <f t="shared" si="4"/>
         <v>2097152</v>
       </c>
       <c r="D142">
@@ -8874,7 +8874,7 @@
         <v>22</v>
       </c>
       <c r="B143">
-        <f>2^A143</f>
+        <f t="shared" si="4"/>
         <v>4194304</v>
       </c>
       <c r="D143">

</xml_diff>